<commit_message>
added ticks to the labels
</commit_message>
<xml_diff>
--- a/CLUSTER-SIZES-0act-cl-n-hcl.xlsx
+++ b/CLUSTER-SIZES-0act-cl-n-hcl.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10307"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/opoku/Desktop/thesis-graph-jupyter/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/opoku/Desktop/Thesis_graphs_binder/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{882C4214-F2F1-1D4B-BD5A-E99D8433173F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{944741D5-D92D-654E-A5B6-EC6753AF5F81}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6820" yWindow="1120" windowWidth="16360" windowHeight="14880" xr2:uid="{66FEA771-CEBD-3F41-A3DD-F4748892B5D8}"/>
+    <workbookView xWindow="3920" yWindow="500" windowWidth="19240" windowHeight="14880" xr2:uid="{66FEA771-CEBD-3F41-A3DD-F4748892B5D8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="28">
   <si>
     <t>noofwater</t>
   </si>
@@ -103,6 +103,12 @@
   </si>
   <si>
     <t>cl_x2c_d_acv4z_2p</t>
+  </si>
+  <si>
+    <t>cl-au</t>
+  </si>
+  <si>
+    <t>hcl-au</t>
   </si>
 </sst>
 </file>
@@ -454,95 +460,155 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55387CED-37BE-2A46-9802-6A940C968A22}">
-  <dimension ref="A1:BD7"/>
+  <dimension ref="A1:AT7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
-      <selection activeCell="AC13" sqref="AC13"/>
+    <sheetView tabSelected="1" topLeftCell="AI1" workbookViewId="0">
+      <selection activeCell="AC1" sqref="AC1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:56" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
+      <c r="B1" t="s">
+        <v>26</v>
+      </c>
       <c r="C1" t="s">
         <v>1</v>
       </c>
+      <c r="D1" t="s">
+        <v>26</v>
+      </c>
       <c r="E1" t="s">
         <v>2</v>
       </c>
       <c r="F1" t="s">
         <v>22</v>
       </c>
+      <c r="G1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H1" t="s">
+        <v>3</v>
+      </c>
       <c r="I1" t="s">
-        <v>3</v>
+        <v>26</v>
+      </c>
+      <c r="J1" t="s">
+        <v>4</v>
       </c>
       <c r="K1" t="s">
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="L1" t="s">
-        <v>21</v>
+        <v>26</v>
+      </c>
+      <c r="M1" t="s">
+        <v>5</v>
+      </c>
+      <c r="N1" t="s">
+        <v>26</v>
+      </c>
+      <c r="O1" t="s">
+        <v>6</v>
       </c>
       <c r="P1" t="s">
-        <v>5</v>
+        <v>23</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>26</v>
       </c>
       <c r="R1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="S1" t="s">
-        <v>23</v>
+        <v>26</v>
+      </c>
+      <c r="T1" t="s">
+        <v>8</v>
+      </c>
+      <c r="U1" t="s">
+        <v>24</v>
       </c>
       <c r="V1" t="s">
-        <v>7</v>
+        <v>26</v>
+      </c>
+      <c r="W1" t="s">
+        <v>9</v>
       </c>
       <c r="X1" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="Y1" t="s">
-        <v>24</v>
+        <v>10</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>27</v>
       </c>
       <c r="AB1" t="s">
-        <v>9</v>
+        <v>11</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>27</v>
       </c>
       <c r="AD1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="AE1" t="s">
-        <v>25</v>
+        <v>27</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>13</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>27</v>
       </c>
       <c r="AH1" t="s">
-        <v>11</v>
+        <v>15</v>
+      </c>
+      <c r="AI1" t="s">
+        <v>27</v>
       </c>
       <c r="AJ1" t="s">
-        <v>12</v>
+        <v>14</v>
+      </c>
+      <c r="AK1" t="s">
+        <v>27</v>
+      </c>
+      <c r="AL1" t="s">
+        <v>16</v>
       </c>
       <c r="AM1" t="s">
-        <v>13</v>
+        <v>27</v>
+      </c>
+      <c r="AN1" t="s">
+        <v>17</v>
       </c>
       <c r="AO1" t="s">
-        <v>15</v>
+        <v>27</v>
+      </c>
+      <c r="AP1" t="s">
+        <v>18</v>
+      </c>
+      <c r="AQ1" t="s">
+        <v>27</v>
       </c>
       <c r="AR1" t="s">
-        <v>14</v>
+        <v>19</v>
+      </c>
+      <c r="AS1" t="s">
+        <v>27</v>
       </c>
       <c r="AT1" t="s">
-        <v>16</v>
-      </c>
-      <c r="AW1" t="s">
-        <v>17</v>
-      </c>
-      <c r="AY1" t="s">
-        <v>18</v>
-      </c>
-      <c r="BB1" t="s">
-        <v>19</v>
-      </c>
-      <c r="BD1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:56" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>0</v>
       </c>
@@ -564,150 +630,150 @@
         <f>(C2+E2)/2</f>
         <v>198.972068348785</v>
       </c>
+      <c r="G2">
+        <v>7.3439220699999996</v>
+      </c>
       <c r="H2">
-        <v>7.3439220699999996</v>
+        <f>27.211*G2</f>
+        <v>199.83546344676998</v>
       </c>
       <c r="I2">
-        <f>27.211*H2</f>
-        <v>199.83546344676998</v>
+        <v>7.2817214200000002</v>
       </c>
       <c r="J2">
-        <v>7.2817214200000002</v>
+        <f>I2*27.211</f>
+        <v>198.14292155961999</v>
       </c>
       <c r="K2">
-        <f>J2*27.211</f>
-        <v>198.14292155961999</v>
+        <f>(H2+J2)/2</f>
+        <v>198.989192503195</v>
       </c>
       <c r="L2">
-        <f>(I2+K2)/2</f>
-        <v>198.989192503195</v>
+        <v>7.3433585600000004</v>
+      </c>
+      <c r="M2">
+        <f>L2*27.211</f>
+        <v>199.82012977616</v>
+      </c>
+      <c r="N2">
+        <v>7.2808410700000001</v>
       </c>
       <c r="O2">
-        <v>7.3433585600000004</v>
+        <f>N2*27.211</f>
+        <v>198.11896635577</v>
       </c>
       <c r="P2">
-        <f>O2*27.211</f>
-        <v>199.82012977616</v>
+        <f>(M2+O2)/2</f>
+        <v>198.969548065965</v>
       </c>
       <c r="Q2">
-        <v>7.2808410700000001</v>
+        <v>7.3435528000000003</v>
       </c>
       <c r="R2">
         <f>Q2*27.211</f>
-        <v>198.11896635577</v>
+        <v>199.8254152408</v>
       </c>
       <c r="S2">
-        <f>(P2+R2)/2</f>
-        <v>198.969548065965</v>
+        <v>7.2812390599999999</v>
+      </c>
+      <c r="T2">
+        <f>S2*27.211</f>
+        <v>198.12979606165999</v>
       </c>
       <c r="U2">
-        <v>7.3435528000000003</v>
+        <f>(R2+T2)/2</f>
+        <v>198.97760565122999</v>
       </c>
       <c r="V2">
-        <f>U2*27.211</f>
-        <v>199.8254152408</v>
+        <v>7.3434169799999998</v>
       </c>
       <c r="W2">
-        <v>7.2812390599999999</v>
+        <f>V2*27.211</f>
+        <v>199.82171944277999</v>
       </c>
       <c r="X2">
-        <f>W2*27.211</f>
-        <v>198.12979606165999</v>
+        <v>7.2809005100000004</v>
       </c>
       <c r="Y2">
-        <f>(V2+X2)/2</f>
-        <v>198.97760565122999</v>
+        <f>X2*27.211</f>
+        <v>198.12058377760999</v>
+      </c>
+      <c r="Z2">
+        <f>(W2+Y2)/2</f>
+        <v>198.97115161019499</v>
       </c>
       <c r="AA2">
-        <v>7.3434169799999998</v>
+        <v>7.7081556999999998</v>
       </c>
       <c r="AB2">
         <f>AA2*27.211</f>
-        <v>199.82171944277999</v>
+        <v>209.74662475269997</v>
       </c>
       <c r="AC2">
-        <v>7.2809005100000004</v>
+        <v>7.6472886600000001</v>
       </c>
       <c r="AD2">
         <f>AC2*27.211</f>
-        <v>198.12058377760999</v>
+        <v>208.09037172725999</v>
       </c>
       <c r="AE2">
-        <f>(AB2+AD2)/2</f>
-        <v>198.97115161019499</v>
+        <v>7.7087324300000004</v>
+      </c>
+      <c r="AF2">
+        <f>AE2*27.211</f>
+        <v>209.76231815272999</v>
       </c>
       <c r="AG2">
-        <v>7.7081556999999998</v>
+        <v>7.6479805399999998</v>
       </c>
       <c r="AH2">
         <f>AG2*27.211</f>
-        <v>209.74662475269997</v>
+        <v>208.10919847393998</v>
       </c>
       <c r="AI2">
-        <v>7.6472886600000001</v>
+        <v>7.7083271499999997</v>
       </c>
       <c r="AJ2">
         <f>AI2*27.211</f>
-        <v>208.09037172725999</v>
+        <v>209.75129007864999</v>
+      </c>
+      <c r="AK2">
+        <v>7.6440204899999999</v>
       </c>
       <c r="AL2">
-        <v>7.7087324300000004</v>
+        <f>AK2*27.211</f>
+        <v>208.00144155338998</v>
       </c>
       <c r="AM2">
-        <f>AL2*27.211</f>
-        <v>209.76231815272999</v>
+        <v>7.7081571699999998</v>
       </c>
       <c r="AN2">
-        <v>7.6479805399999998</v>
+        <f>AM2*27.211</f>
+        <v>209.74666475286998</v>
       </c>
       <c r="AO2">
-        <f>AN2*27.211</f>
-        <v>208.10919847393998</v>
+        <v>7.6472889799999999</v>
+      </c>
+      <c r="AP2">
+        <f>AO2*27.211</f>
+        <v>208.09038043477997</v>
       </c>
       <c r="AQ2">
-        <v>7.7083271499999997</v>
+        <v>7.7082934200000004</v>
       </c>
       <c r="AR2">
         <f>AQ2*27.211</f>
-        <v>209.75129007864999</v>
+        <v>209.75037225162001</v>
       </c>
       <c r="AS2">
-        <v>7.6440204899999999</v>
+        <v>7.6439992999999999</v>
       </c>
       <c r="AT2">
         <f>AS2*27.211</f>
-        <v>208.00144155338998</v>
-      </c>
-      <c r="AV2">
-        <v>7.7081571699999998</v>
-      </c>
-      <c r="AW2">
-        <f>AV2*27.211</f>
-        <v>209.74666475286998</v>
-      </c>
-      <c r="AX2">
-        <v>7.6472889799999999</v>
-      </c>
-      <c r="AY2">
-        <f>AX2*27.211</f>
-        <v>208.09038043477997</v>
-      </c>
-      <c r="BA2">
-        <v>7.7082934200000004</v>
-      </c>
-      <c r="BB2">
-        <f>BA2*27.211</f>
-        <v>209.75037225162001</v>
-      </c>
-      <c r="BC2">
-        <v>7.6439992999999999</v>
-      </c>
-      <c r="BD2">
-        <f>BC2*27.211</f>
         <v>208.00086495229999</v>
       </c>
     </row>
-    <row r="3" spans="1:56" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>7</v>
       </c>
@@ -729,150 +795,150 @@
         <f t="shared" ref="F3:F7" si="2">(C3+E3)/2</f>
         <v>199.33354798030501</v>
       </c>
+      <c r="G3">
+        <v>7.3572208100000003</v>
+      </c>
       <c r="H3">
-        <v>7.3572208100000003</v>
+        <f t="shared" ref="H3:H7" si="3">27.211*G3</f>
+        <v>200.19733546090998</v>
       </c>
       <c r="I3">
-        <f t="shared" ref="I3:I7" si="3">27.211*H3</f>
-        <v>200.19733546090998</v>
+        <v>7.2949913300000002</v>
       </c>
       <c r="J3">
-        <v>7.2949913300000002</v>
+        <f t="shared" ref="J3:J7" si="4">I3*27.211</f>
+        <v>198.50400908063</v>
       </c>
       <c r="K3">
-        <f t="shared" ref="K3:K7" si="4">J3*27.211</f>
-        <v>198.50400908063</v>
+        <f t="shared" ref="K3:K7" si="5">(H3+J3)/2</f>
+        <v>199.35067227076999</v>
       </c>
       <c r="L3">
-        <f t="shared" ref="L3:L7" si="5">(I3+K3)/2</f>
-        <v>199.35067227076999</v>
+        <v>7.35696101</v>
+      </c>
+      <c r="M3">
+        <f t="shared" ref="M3:M7" si="6">L3*27.211</f>
+        <v>200.19026604311</v>
+      </c>
+      <c r="N3">
+        <v>7.2944241999999999</v>
       </c>
       <c r="O3">
-        <v>7.35696101</v>
+        <f t="shared" ref="O3:O7" si="7">N3*27.211</f>
+        <v>198.4885769062</v>
       </c>
       <c r="P3">
-        <f t="shared" ref="P3:P7" si="6">O3*27.211</f>
-        <v>200.19026604311</v>
+        <f t="shared" ref="P3:P7" si="8">(M3+O3)/2</f>
+        <v>199.33942147465501</v>
       </c>
       <c r="Q3">
-        <v>7.2944241999999999</v>
+        <v>7.3575945100000002</v>
       </c>
       <c r="R3">
-        <f t="shared" ref="R3:R7" si="7">Q3*27.211</f>
-        <v>198.4885769062</v>
+        <f t="shared" ref="R3:R7" si="9">Q3*27.211</f>
+        <v>200.20750421161</v>
       </c>
       <c r="S3">
-        <f t="shared" ref="S3:S7" si="8">(P3+R3)/2</f>
-        <v>199.33942147465501</v>
+        <v>7.2952567699999999</v>
+      </c>
+      <c r="T3">
+        <f t="shared" ref="T3:T7" si="10">S3*27.211</f>
+        <v>198.51123196846999</v>
       </c>
       <c r="U3">
-        <v>7.3575945100000002</v>
+        <f t="shared" ref="U3:U7" si="11">(R3+T3)/2</f>
+        <v>199.35936809003999</v>
       </c>
       <c r="V3">
-        <f t="shared" ref="V3:V7" si="9">U3*27.211</f>
-        <v>200.20750421161</v>
+        <v>7.3577189599999997</v>
       </c>
       <c r="W3">
-        <v>7.2952567699999999</v>
+        <f t="shared" ref="W3:W7" si="12">V3*27.211</f>
+        <v>200.21089062055998</v>
       </c>
       <c r="X3">
-        <f t="shared" ref="X3:X7" si="10">W3*27.211</f>
-        <v>198.51123196846999</v>
+        <v>7.2951825000000001</v>
       </c>
       <c r="Y3">
-        <f t="shared" ref="Y3:Y7" si="11">(V3+X3)/2</f>
-        <v>199.35936809003999</v>
+        <f t="shared" ref="Y3:Y7" si="13">X3*27.211</f>
+        <v>198.5092110075</v>
+      </c>
+      <c r="Z3">
+        <f t="shared" ref="Z3:Z7" si="14">(W3+Y3)/2</f>
+        <v>199.36005081402999</v>
       </c>
       <c r="AA3">
-        <v>7.3577189599999997</v>
+        <v>7.7003628400000004</v>
       </c>
       <c r="AB3">
-        <f t="shared" ref="AB3:AB7" si="12">AA3*27.211</f>
-        <v>200.21089062055998</v>
+        <f t="shared" ref="AB3:AB7" si="15">AA3*27.211</f>
+        <v>209.53457323923999</v>
       </c>
       <c r="AC3">
-        <v>7.2951825000000001</v>
+        <v>7.6394248899999999</v>
       </c>
       <c r="AD3">
-        <f t="shared" ref="AD3:AD7" si="13">AC3*27.211</f>
-        <v>198.5092110075</v>
+        <f t="shared" ref="AD3:AD7" si="16">AC3*27.211</f>
+        <v>207.87639068178999</v>
       </c>
       <c r="AE3">
-        <f t="shared" ref="AE3:AE7" si="14">(AB3+AD3)/2</f>
-        <v>199.36005081402999</v>
+        <v>7.7009384499999998</v>
+      </c>
+      <c r="AF3">
+        <f t="shared" ref="AF3:AF7" si="17">AE3*27.211</f>
+        <v>209.55023616294997</v>
       </c>
       <c r="AG3">
-        <v>7.7003628400000004</v>
+        <v>7.6401160900000002</v>
       </c>
       <c r="AH3">
-        <f t="shared" ref="AH3:AH7" si="15">AG3*27.211</f>
-        <v>209.53457323923999</v>
+        <f t="shared" ref="AH3:AH7" si="18">AG3*27.211</f>
+        <v>207.89519892498998</v>
       </c>
       <c r="AI3">
-        <v>7.6394248899999999</v>
+        <v>7.7005957799999996</v>
       </c>
       <c r="AJ3">
-        <f t="shared" ref="AJ3:AJ7" si="16">AI3*27.211</f>
-        <v>207.87639068178999</v>
+        <f t="shared" ref="AJ3:AJ7" si="19">AI3*27.211</f>
+        <v>209.54091176957996</v>
+      </c>
+      <c r="AK3">
+        <v>7.6395744700000003</v>
       </c>
       <c r="AL3">
-        <v>7.7009384499999998</v>
+        <f t="shared" ref="AL3:AL7" si="20">AK3*27.211</f>
+        <v>207.88046090316999</v>
       </c>
       <c r="AM3">
-        <f t="shared" ref="AM3:AM7" si="17">AL3*27.211</f>
-        <v>209.55023616294997</v>
+        <v>7.7004235999999997</v>
       </c>
       <c r="AN3">
-        <v>7.6401160900000002</v>
+        <f t="shared" ref="AN3:AN7" si="21">AM3*27.211</f>
+        <v>209.53622657959997</v>
       </c>
       <c r="AO3">
-        <f t="shared" ref="AO3:AO7" si="18">AN3*27.211</f>
-        <v>207.89519892498998</v>
+        <v>7.6394847400000003</v>
+      </c>
+      <c r="AP3">
+        <f t="shared" ref="AP3:AP7" si="22">AO3*27.211</f>
+        <v>207.87801926014001</v>
       </c>
       <c r="AQ3">
-        <v>7.7005957799999996</v>
+        <v>7.7006237200000003</v>
       </c>
       <c r="AR3">
-        <f t="shared" ref="AR3:AR7" si="19">AQ3*27.211</f>
-        <v>209.54091176957996</v>
+        <f t="shared" ref="AR3:AR7" si="23">AQ3*27.211</f>
+        <v>209.54167204492001</v>
       </c>
       <c r="AS3">
-        <v>7.6395744700000003</v>
+        <v>7.6395936400000002</v>
       </c>
       <c r="AT3">
-        <f t="shared" ref="AT3:AT7" si="20">AS3*27.211</f>
-        <v>207.88046090316999</v>
-      </c>
-      <c r="AV3">
-        <v>7.7004235999999997</v>
-      </c>
-      <c r="AW3">
-        <f t="shared" ref="AW3:AW7" si="21">AV3*27.211</f>
-        <v>209.53622657959997</v>
-      </c>
-      <c r="AX3">
-        <v>7.6394847400000003</v>
-      </c>
-      <c r="AY3">
-        <f t="shared" ref="AY3:AY7" si="22">AX3*27.211</f>
-        <v>207.87801926014001</v>
-      </c>
-      <c r="BA3">
-        <v>7.7006237200000003</v>
-      </c>
-      <c r="BB3">
-        <f t="shared" ref="BB3:BB7" si="23">BA3*27.211</f>
-        <v>209.54167204492001</v>
-      </c>
-      <c r="BC3">
-        <v>7.6395936400000002</v>
-      </c>
-      <c r="BD3">
-        <f t="shared" ref="BD3:BD7" si="24">BC3*27.211</f>
+        <f t="shared" ref="AT3:AT7" si="24">AS3*27.211</f>
         <v>207.88098253804</v>
       </c>
     </row>
-    <row r="4" spans="1:56" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>49</v>
       </c>
@@ -894,150 +960,150 @@
         <f t="shared" si="2"/>
         <v>199.52589097462999</v>
       </c>
+      <c r="G4">
+        <v>7.3642989300000004</v>
+      </c>
       <c r="H4">
-        <v>7.3642989300000004</v>
-      </c>
-      <c r="I4">
         <f t="shared" si="3"/>
         <v>200.38993818423</v>
       </c>
+      <c r="I4">
+        <v>7.3020504700000002</v>
+      </c>
       <c r="J4">
-        <v>7.3020504700000002</v>
-      </c>
-      <c r="K4">
         <f t="shared" si="4"/>
         <v>198.69609533917</v>
       </c>
-      <c r="L4">
+      <c r="K4">
         <f t="shared" si="5"/>
         <v>199.54301676170002</v>
       </c>
-      <c r="O4">
+      <c r="L4">
         <v>7.3641292299999996</v>
       </c>
-      <c r="P4">
+      <c r="M4">
         <f t="shared" si="6"/>
         <v>200.38532047752997</v>
       </c>
-      <c r="Q4">
+      <c r="N4">
         <v>7.3015785199999996</v>
       </c>
-      <c r="R4">
+      <c r="O4">
         <f t="shared" si="7"/>
         <v>198.68325310771999</v>
       </c>
-      <c r="S4">
+      <c r="P4">
         <f t="shared" si="8"/>
         <v>199.53428679262498</v>
       </c>
-      <c r="U4">
+      <c r="Q4">
         <v>7.3649102700000002</v>
       </c>
-      <c r="V4">
+      <c r="R4">
         <f t="shared" si="9"/>
         <v>200.40657335697</v>
       </c>
-      <c r="W4">
+      <c r="S4">
         <v>7.3025559500000004</v>
       </c>
-      <c r="X4">
+      <c r="T4">
         <f t="shared" si="10"/>
         <v>198.70984995545001</v>
       </c>
-      <c r="Y4">
+      <c r="U4">
         <f t="shared" si="11"/>
         <v>199.55821165621001</v>
       </c>
-      <c r="AA4">
+      <c r="V4">
         <v>7.3650395099999999</v>
       </c>
-      <c r="AB4">
+      <c r="W4">
         <f t="shared" si="12"/>
         <v>200.41009010661</v>
       </c>
-      <c r="AC4">
+      <c r="X4">
         <v>7.3024892399999999</v>
       </c>
-      <c r="AD4">
+      <c r="Y4">
         <f t="shared" si="13"/>
         <v>198.70803470963997</v>
       </c>
-      <c r="AE4">
+      <c r="Z4">
         <f t="shared" si="14"/>
         <v>199.55906240812499</v>
       </c>
-      <c r="AG4">
+      <c r="AA4">
         <v>7.70091474</v>
       </c>
-      <c r="AH4">
+      <c r="AB4">
         <f t="shared" si="15"/>
         <v>209.54959099013999</v>
       </c>
-      <c r="AI4">
+      <c r="AC4">
         <v>7.6399566099999996</v>
       </c>
-      <c r="AJ4">
+      <c r="AD4">
         <f t="shared" si="16"/>
         <v>207.89085931470999</v>
       </c>
-      <c r="AL4">
+      <c r="AE4">
         <v>7.7014901499999997</v>
       </c>
-      <c r="AM4">
+      <c r="AF4">
         <f t="shared" si="17"/>
         <v>209.56524847164999</v>
       </c>
-      <c r="AN4">
+      <c r="AG4">
         <v>7.64064765</v>
       </c>
-      <c r="AO4">
+      <c r="AH4">
         <f t="shared" si="18"/>
         <v>207.90966320414998</v>
       </c>
-      <c r="AQ4">
+      <c r="AI4">
         <v>7.7011516499999999</v>
       </c>
-      <c r="AR4">
+      <c r="AJ4">
         <f t="shared" si="19"/>
         <v>209.55603754814999</v>
       </c>
-      <c r="AS4">
+      <c r="AK4">
         <v>7.6401132</v>
       </c>
-      <c r="AT4">
+      <c r="AL4">
         <f t="shared" si="20"/>
         <v>207.89512028519999</v>
       </c>
-      <c r="AV4">
+      <c r="AM4">
         <v>7.7009854000000004</v>
       </c>
-      <c r="AW4">
+      <c r="AN4">
         <f t="shared" si="21"/>
         <v>209.55151371939999</v>
       </c>
-      <c r="AX4">
+      <c r="AO4">
         <v>7.6400266600000002</v>
       </c>
-      <c r="AY4">
+      <c r="AP4">
         <f t="shared" si="22"/>
         <v>207.89276544525998</v>
       </c>
-      <c r="BA4">
+      <c r="AQ4">
         <v>7.7011811300000002</v>
       </c>
-      <c r="BB4">
+      <c r="AR4">
         <f t="shared" si="23"/>
         <v>209.55683972842999</v>
       </c>
-      <c r="BC4">
+      <c r="AS4">
         <v>7.6401338399999998</v>
       </c>
-      <c r="BD4">
+      <c r="AT4">
         <f t="shared" si="24"/>
         <v>207.89568192023998</v>
       </c>
     </row>
-    <row r="5" spans="1:56" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>99</v>
       </c>
@@ -1059,150 +1125,150 @@
         <f t="shared" si="2"/>
         <v>199.57519921139999</v>
       </c>
+      <c r="G5">
+        <v>7.3661117200000001</v>
+      </c>
       <c r="H5">
-        <v>7.3661117200000001</v>
-      </c>
-      <c r="I5">
         <f t="shared" si="3"/>
         <v>200.43926601292</v>
       </c>
+      <c r="I5">
+        <v>7.3038618499999997</v>
+      </c>
       <c r="J5">
-        <v>7.3038618499999997</v>
-      </c>
-      <c r="K5">
         <f t="shared" si="4"/>
         <v>198.74538480034997</v>
       </c>
-      <c r="L5">
+      <c r="K5">
         <f t="shared" si="5"/>
         <v>199.59232540663498</v>
       </c>
-      <c r="O5">
+      <c r="L5">
         <v>7.3659621599999996</v>
       </c>
-      <c r="P5">
+      <c r="M5">
         <f t="shared" si="6"/>
         <v>200.43519633575997</v>
       </c>
-      <c r="Q5">
+      <c r="N5">
         <v>7.30341036</v>
       </c>
-      <c r="R5">
+      <c r="O5">
         <f t="shared" si="7"/>
         <v>198.73309930596</v>
       </c>
-      <c r="S5">
+      <c r="P5">
         <f t="shared" si="8"/>
         <v>199.58414782085998</v>
       </c>
-      <c r="U5">
+      <c r="Q5">
         <v>7.3667680999999998</v>
       </c>
-      <c r="V5">
+      <c r="R5">
         <f t="shared" si="9"/>
         <v>200.45712676909997</v>
       </c>
-      <c r="W5">
+      <c r="S5">
         <v>7.3044124699999999</v>
       </c>
-      <c r="X5">
+      <c r="T5">
         <f t="shared" si="10"/>
         <v>198.76036772116998</v>
       </c>
-      <c r="Y5">
+      <c r="U5">
         <f t="shared" si="11"/>
         <v>199.60874724513496</v>
       </c>
-      <c r="AA5">
+      <c r="V5">
         <v>7.3668884500000003</v>
       </c>
-      <c r="AB5">
+      <c r="W5">
         <f t="shared" si="12"/>
         <v>200.46040161294999</v>
       </c>
-      <c r="AC5">
+      <c r="X5">
         <v>7.3043370699999999</v>
       </c>
-      <c r="AD5">
+      <c r="Y5">
         <f t="shared" si="13"/>
         <v>198.75831601176998</v>
       </c>
-      <c r="AE5">
+      <c r="Z5">
         <f t="shared" si="14"/>
         <v>199.60935881235997</v>
       </c>
-      <c r="AG5">
+      <c r="AA5">
         <v>7.7015783200000003</v>
       </c>
-      <c r="AH5">
+      <c r="AB5">
         <f t="shared" si="15"/>
         <v>209.56764766551998</v>
       </c>
-      <c r="AI5">
+      <c r="AC5">
         <v>7.6406183700000003</v>
       </c>
-      <c r="AJ5">
+      <c r="AD5">
         <f t="shared" si="16"/>
         <v>207.90886646607001</v>
       </c>
-      <c r="AL5">
+      <c r="AE5">
         <v>7.7021536900000003</v>
       </c>
-      <c r="AM5">
+      <c r="AF5">
         <f t="shared" si="17"/>
         <v>209.58330405858999</v>
       </c>
-      <c r="AN5">
+      <c r="AG5">
         <v>7.64130939</v>
       </c>
-      <c r="AO5">
+      <c r="AH5">
         <f t="shared" si="18"/>
         <v>207.92766981129</v>
       </c>
-      <c r="AQ5">
+      <c r="AI5">
         <v>7.7018167999999996</v>
       </c>
-      <c r="AR5">
+      <c r="AJ5">
         <f t="shared" si="19"/>
         <v>209.57413694479999</v>
       </c>
-      <c r="AS5">
+      <c r="AK5">
         <v>7.6407767599999996</v>
       </c>
-      <c r="AT5">
+      <c r="AL5">
         <f t="shared" si="20"/>
         <v>207.91317641635999</v>
       </c>
-      <c r="AV5">
+      <c r="AM5">
         <v>7.7016515099999996</v>
       </c>
-      <c r="AW5">
+      <c r="AN5">
         <f t="shared" si="21"/>
         <v>209.56963923860997</v>
       </c>
-      <c r="AX5">
+      <c r="AO5">
         <v>7.6406909599999997</v>
       </c>
-      <c r="AY5">
+      <c r="AP5">
         <f t="shared" si="22"/>
         <v>207.91084171255997</v>
       </c>
-      <c r="BA5">
+      <c r="AQ5">
         <v>7.7018465999999997</v>
       </c>
-      <c r="BB5">
+      <c r="AR5">
         <f t="shared" si="23"/>
         <v>209.57494783259997</v>
       </c>
-      <c r="BC5">
+      <c r="AS5">
         <v>7.6407977100000002</v>
       </c>
-      <c r="BD5">
+      <c r="AT5">
         <f t="shared" si="24"/>
         <v>207.91374648681</v>
       </c>
     </row>
-    <row r="6" spans="1:56" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>149</v>
       </c>
@@ -1224,150 +1290,150 @@
         <f t="shared" si="2"/>
         <v>199.31587538818999</v>
       </c>
+      <c r="G6">
+        <v>7.3565812099999999</v>
+      </c>
       <c r="H6">
-        <v>7.3565812099999999</v>
-      </c>
-      <c r="I6">
         <f t="shared" si="3"/>
         <v>200.17993130530999</v>
       </c>
+      <c r="I6">
+        <v>7.29433211</v>
+      </c>
       <c r="J6">
-        <v>7.29433211</v>
-      </c>
-      <c r="K6">
         <f t="shared" si="4"/>
         <v>198.48607104521</v>
       </c>
-      <c r="L6">
+      <c r="K6">
         <f t="shared" si="5"/>
         <v>199.33300117525999</v>
       </c>
-      <c r="O6">
+      <c r="L6">
         <v>7.3564252200000002</v>
       </c>
-      <c r="P6">
+      <c r="M6">
         <f t="shared" si="6"/>
         <v>200.17568666142</v>
       </c>
-      <c r="Q6">
+      <c r="N6">
         <v>7.2938739799999999</v>
       </c>
-      <c r="R6">
+      <c r="O6">
         <f t="shared" si="7"/>
         <v>198.47360486977999</v>
       </c>
-      <c r="S6">
+      <c r="P6">
         <f t="shared" si="8"/>
         <v>199.3246457656</v>
       </c>
-      <c r="U6">
+      <c r="Q6">
         <v>7.3572258899999996</v>
       </c>
-      <c r="V6">
+      <c r="R6">
         <f t="shared" si="9"/>
         <v>200.19747369278997</v>
       </c>
-      <c r="W6">
+      <c r="S6">
         <v>7.2948709599999999</v>
       </c>
-      <c r="X6">
+      <c r="T6">
         <f t="shared" si="10"/>
         <v>198.50073369255998</v>
       </c>
-      <c r="Y6">
+      <c r="U6">
         <f t="shared" si="11"/>
         <v>199.34910369267499</v>
       </c>
-      <c r="AA6">
+      <c r="V6">
         <v>7.3573424200000002</v>
       </c>
-      <c r="AB6">
+      <c r="W6">
         <f t="shared" si="12"/>
         <v>200.20064459061999</v>
       </c>
-      <c r="AC6">
+      <c r="X6">
         <v>7.2947916099999999</v>
       </c>
-      <c r="AD6">
+      <c r="Y6">
         <f t="shared" si="13"/>
         <v>198.49857449970997</v>
       </c>
-      <c r="AE6">
+      <c r="Z6">
         <f t="shared" si="14"/>
         <v>199.34960954516498</v>
       </c>
-      <c r="AG6">
+      <c r="AA6">
         <v>7.6936690700000003</v>
       </c>
-      <c r="AH6">
+      <c r="AB6">
         <f t="shared" si="15"/>
         <v>209.35242906376999</v>
       </c>
-      <c r="AI6">
+      <c r="AC6">
         <v>7.6327108299999997</v>
       </c>
-      <c r="AJ6">
+      <c r="AD6">
         <f t="shared" si="16"/>
         <v>207.69369439513</v>
       </c>
-      <c r="AL6">
+      <c r="AE6">
         <v>7.6942444700000001</v>
       </c>
-      <c r="AM6">
+      <c r="AF6">
         <f t="shared" si="17"/>
         <v>209.36808627316998</v>
       </c>
-      <c r="AN6">
+      <c r="AG6">
         <v>7.6334018700000001</v>
       </c>
-      <c r="AO6">
+      <c r="AH6">
         <f t="shared" si="18"/>
         <v>207.71249828456999</v>
       </c>
-      <c r="AQ6">
+      <c r="AI6">
         <v>7.6939072099999999</v>
       </c>
-      <c r="AR6">
+      <c r="AJ6">
         <f t="shared" si="19"/>
         <v>209.35890909130998</v>
       </c>
-      <c r="AS6">
+      <c r="AK6">
         <v>7.6328686399999999</v>
       </c>
-      <c r="AT6">
+      <c r="AL6">
         <f t="shared" si="20"/>
         <v>207.69798856303998</v>
       </c>
-      <c r="AV6">
+      <c r="AM6">
         <v>7.6937416499999998</v>
       </c>
-      <c r="AW6">
+      <c r="AN6">
         <f t="shared" si="21"/>
         <v>209.35440403814999</v>
       </c>
-      <c r="AX6">
+      <c r="AO6">
         <v>7.6327828000000002</v>
       </c>
-      <c r="AY6">
+      <c r="AP6">
         <f t="shared" si="22"/>
         <v>207.6956527708</v>
       </c>
-      <c r="BA6">
+      <c r="AQ6">
         <v>7.6939364899999996</v>
       </c>
-      <c r="BB6">
+      <c r="AR6">
         <f t="shared" si="23"/>
         <v>209.35970582938998</v>
       </c>
-      <c r="BC6">
+      <c r="AS6">
         <v>7.63288908</v>
       </c>
-      <c r="BD6">
+      <c r="AT6">
         <f t="shared" si="24"/>
         <v>207.69854475587999</v>
       </c>
     </row>
-    <row r="7" spans="1:56" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>199</v>
       </c>
@@ -1389,145 +1455,145 @@
         <f t="shared" si="2"/>
         <v>199.35924795347501</v>
       </c>
+      <c r="G7">
+        <v>7.35817517</v>
+      </c>
       <c r="H7">
-        <v>7.35817517</v>
-      </c>
-      <c r="I7">
         <f t="shared" si="3"/>
         <v>200.22330455086998</v>
       </c>
+      <c r="I7">
+        <v>7.2959260400000003</v>
+      </c>
       <c r="J7">
-        <v>7.2959260400000003</v>
-      </c>
-      <c r="K7">
         <f t="shared" si="4"/>
         <v>198.52944347444</v>
       </c>
-      <c r="L7">
+      <c r="K7">
         <f t="shared" si="5"/>
         <v>199.37637401265499</v>
       </c>
-      <c r="O7">
+      <c r="L7">
         <v>7.3580270900000002</v>
       </c>
-      <c r="P7">
+      <c r="M7">
         <f t="shared" si="6"/>
         <v>200.21927514599</v>
       </c>
-      <c r="Q7">
+      <c r="N7">
         <v>7.2954757900000002</v>
       </c>
-      <c r="R7">
+      <c r="O7">
         <f t="shared" si="7"/>
         <v>198.51719172168998</v>
       </c>
-      <c r="S7">
+      <c r="P7">
         <f t="shared" si="8"/>
         <v>199.36823343383998</v>
       </c>
-      <c r="U7">
+      <c r="Q7">
         <v>7.3588339100000004</v>
       </c>
-      <c r="V7">
+      <c r="R7">
         <f t="shared" si="9"/>
         <v>200.24122952501</v>
       </c>
-      <c r="W7">
+      <c r="S7">
         <v>7.2964789100000003</v>
       </c>
-      <c r="X7">
+      <c r="T7">
         <f t="shared" si="10"/>
         <v>198.54448762000999</v>
       </c>
-      <c r="Y7">
+      <c r="U7">
         <f t="shared" si="11"/>
         <v>199.39285857250999</v>
       </c>
-      <c r="AA7">
+      <c r="V7">
         <v>7.35894812</v>
       </c>
-      <c r="AB7">
+      <c r="W7">
         <f t="shared" si="12"/>
         <v>200.24433729332</v>
       </c>
-      <c r="AC7">
+      <c r="X7">
         <v>7.2963972200000002</v>
       </c>
-      <c r="AD7">
+      <c r="Y7">
         <f t="shared" si="13"/>
         <v>198.54226475342</v>
       </c>
-      <c r="AE7">
+      <c r="Z7">
         <f t="shared" si="14"/>
         <v>199.39330102336999</v>
       </c>
-      <c r="AG7">
+      <c r="AA7">
         <v>7.6951616300000003</v>
       </c>
-      <c r="AH7">
+      <c r="AB7">
         <f t="shared" si="15"/>
         <v>209.39304311392999</v>
       </c>
-      <c r="AI7">
+      <c r="AC7">
         <v>7.6342021200000003</v>
       </c>
-      <c r="AJ7">
+      <c r="AD7">
         <f t="shared" si="16"/>
         <v>207.73427388732</v>
       </c>
-      <c r="AL7">
+      <c r="AE7">
         <v>7.6957370100000002</v>
       </c>
-      <c r="AM7">
+      <c r="AF7">
         <f t="shared" si="17"/>
         <v>209.40869977910998</v>
       </c>
-      <c r="AN7">
+      <c r="AG7">
         <v>7.63489314</v>
       </c>
-      <c r="AO7">
+      <c r="AH7">
         <f t="shared" si="18"/>
         <v>207.75307723253999</v>
       </c>
-      <c r="AQ7">
+      <c r="AI7">
         <v>7.6954002600000004</v>
       </c>
-      <c r="AR7">
+      <c r="AJ7">
         <f t="shared" si="19"/>
         <v>209.39953647486001</v>
       </c>
-      <c r="AS7">
+      <c r="AK7">
         <v>7.6343605800000001</v>
       </c>
-      <c r="AT7">
+      <c r="AL7">
         <f t="shared" si="20"/>
         <v>207.73858574238</v>
       </c>
-      <c r="AV7">
+      <c r="AM7">
         <v>7.69523519</v>
       </c>
-      <c r="AW7">
+      <c r="AN7">
         <f t="shared" si="21"/>
         <v>209.39504475509</v>
       </c>
-      <c r="AX7">
+      <c r="AO7">
         <v>7.6342750600000002</v>
       </c>
-      <c r="AY7">
+      <c r="AP7">
         <f t="shared" si="22"/>
         <v>207.73625865765999</v>
       </c>
-      <c r="BA7">
+      <c r="AQ7">
         <v>7.6954299500000003</v>
       </c>
-      <c r="BB7">
+      <c r="AR7">
         <f t="shared" si="23"/>
         <v>209.40034436945001</v>
       </c>
-      <c r="BC7">
+      <c r="AS7">
         <v>7.6343814200000004</v>
       </c>
-      <c r="BD7">
+      <c r="AT7">
         <f t="shared" si="24"/>
         <v>207.73915281961999</v>
       </c>

</xml_diff>

<commit_message>
added 1s, 2s, 2p of HCl
</commit_message>
<xml_diff>
--- a/CLUSTER-SIZES-0act-cl-n-hcl.xlsx
+++ b/CLUSTER-SIZES-0act-cl-n-hcl.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/opoku/Desktop/Thesis_graphs_binder/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/opoku/Desktop/HCl_project_graphs_binder/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A85BDCD-7AC2-B34C-9755-BB84AC624ED5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6F75C48-434F-3746-B42B-DFB2F87A5523}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="440" yWindow="12460" windowWidth="19240" windowHeight="14880" xr2:uid="{66FEA771-CEBD-3F41-A3DD-F4748892B5D8}"/>
+    <workbookView xWindow="-400" yWindow="460" windowWidth="13600" windowHeight="8620" xr2:uid="{66FEA771-CEBD-3F41-A3DD-F4748892B5D8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>noofwater</t>
   </si>
@@ -58,16 +58,59 @@
   </si>
   <si>
     <t>zero_cl_zora_2p32</t>
+  </si>
+  <si>
+    <t>cl_x2c_acv3z_1s</t>
+  </si>
+  <si>
+    <t>cl_x2c_acv3z_2s</t>
+  </si>
+  <si>
+    <t>zero_hcl_zora_1s</t>
+  </si>
+  <si>
+    <t>zero_hcl_zora_2s</t>
+  </si>
+  <si>
+    <t>zero_hcl_zora_2p12</t>
+  </si>
+  <si>
+    <t>zero_hcl_zora_2p32</t>
+  </si>
+  <si>
+    <t>zero_hcl_zora_2p</t>
+  </si>
+  <si>
+    <t>hcl_x2c_acv3z_1s</t>
+  </si>
+  <si>
+    <t>hcl_x2c_acv3z_2s</t>
+  </si>
+  <si>
+    <t>hcl_x2c_acv3z_2p_1half</t>
+  </si>
+  <si>
+    <t>hcl_x2c_acv3z_2p_3half</t>
+  </si>
+  <si>
+    <t>hcl_x2c_acv3z_2p</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -93,8 +136,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -409,15 +453,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55387CED-37BE-2A46-9802-6A940C968A22}">
-  <dimension ref="A1:K7"/>
+  <dimension ref="A1:W7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
+      <selection activeCell="X9" sqref="X9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -437,22 +481,58 @@
         <v>8</v>
       </c>
       <c r="G1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I1" t="s">
         <v>4</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>1</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>5</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
         <v>2</v>
       </c>
-      <c r="K1" t="s">
+      <c r="M1" t="s">
         <v>3</v>
       </c>
+      <c r="N1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="U1" t="s">
+        <v>20</v>
+      </c>
+      <c r="V1" t="s">
+        <v>21</v>
+      </c>
+      <c r="W1" t="s">
+        <v>22</v>
+      </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>0</v>
       </c>
@@ -472,25 +552,62 @@
         <v>183.19</v>
       </c>
       <c r="G2">
+        <v>2824.94</v>
+      </c>
+      <c r="H2">
+        <v>270.33999999999997</v>
+      </c>
+      <c r="I2">
         <v>7.3433493500000004</v>
-      </c>
-      <c r="H2">
-        <f>G2*27.211</f>
-        <v>199.81987916285001</v>
-      </c>
-      <c r="I2">
-        <v>7.2810355199999997</v>
       </c>
       <c r="J2">
         <f>I2*27.211</f>
+        <v>199.81987916285001</v>
+      </c>
+      <c r="K2">
+        <v>7.2810355199999997</v>
+      </c>
+      <c r="L2">
+        <f>K2*27.211</f>
         <v>198.12425753471999</v>
       </c>
-      <c r="K2">
-        <f>(H2+J2)/2</f>
+      <c r="M2">
+        <f>(J2+L2)/2</f>
         <v>198.972068348785</v>
       </c>
+      <c r="N2">
+        <v>2764.75</v>
+      </c>
+      <c r="O2">
+        <v>254.19</v>
+      </c>
+      <c r="P2">
+        <v>194.07</v>
+      </c>
+      <c r="Q2">
+        <v>192.38</v>
+      </c>
+      <c r="R2">
+        <v>193.23</v>
+      </c>
+      <c r="S2">
+        <v>2834.68</v>
+      </c>
+      <c r="T2">
+        <v>280.3</v>
+      </c>
+      <c r="U2">
+        <v>209.74</v>
+      </c>
+      <c r="V2">
+        <v>208.08</v>
+      </c>
+      <c r="W2">
+        <f>(U2+V2)/2</f>
+        <v>208.91000000000003</v>
+      </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>7</v>
       </c>
@@ -510,25 +627,62 @@
         <v>183.73</v>
       </c>
       <c r="G3">
+        <v>2825.73</v>
+      </c>
+      <c r="H3">
+        <v>271.13</v>
+      </c>
+      <c r="I3">
         <v>7.3566480800000003</v>
       </c>
-      <c r="H3">
-        <f t="shared" ref="H3:H7" si="0">G3*27.211</f>
+      <c r="J3">
+        <f t="shared" ref="J3:J7" si="0">I3*27.211</f>
         <v>200.18175090488</v>
       </c>
-      <c r="I3">
+      <c r="K3">
         <v>7.2943054299999996</v>
       </c>
-      <c r="J3">
-        <f t="shared" ref="J3:J7" si="1">I3*27.211</f>
+      <c r="L3">
+        <f t="shared" ref="L3:L7" si="1">K3*27.211</f>
         <v>198.48534505572999</v>
       </c>
-      <c r="K3">
-        <f t="shared" ref="K3:K7" si="2">(H3+J3)/2</f>
+      <c r="M3">
+        <f t="shared" ref="M3:M7" si="2">(J3+L3)/2</f>
         <v>199.33354798030501</v>
       </c>
+      <c r="N3">
+        <v>2764.75</v>
+      </c>
+      <c r="O3">
+        <v>254.09</v>
+      </c>
+      <c r="P3">
+        <v>194.26</v>
+      </c>
+      <c r="Q3">
+        <v>192.56</v>
+      </c>
+      <c r="R3">
+        <v>193.41</v>
+      </c>
+      <c r="S3">
+        <v>2834.81</v>
+      </c>
+      <c r="T3">
+        <v>280.45999999999998</v>
+      </c>
+      <c r="U3">
+        <v>209.52</v>
+      </c>
+      <c r="V3">
+        <v>207.86</v>
+      </c>
+      <c r="W3">
+        <f t="shared" ref="W3:W7" si="3">(U3+V3)/2</f>
+        <v>208.69</v>
+      </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>49</v>
       </c>
@@ -548,25 +702,62 @@
         <v>184</v>
       </c>
       <c r="G4">
+        <v>2825.92</v>
+      </c>
+      <c r="H4">
+        <v>271.32</v>
+      </c>
+      <c r="I4">
         <v>7.3637261199999999</v>
       </c>
-      <c r="H4">
+      <c r="J4">
         <f t="shared" si="0"/>
         <v>200.37435145132</v>
       </c>
-      <c r="I4">
+      <c r="K4">
         <v>7.3013645399999998</v>
       </c>
-      <c r="J4">
+      <c r="L4">
         <f t="shared" si="1"/>
         <v>198.67743049793998</v>
       </c>
-      <c r="K4">
+      <c r="M4">
         <f t="shared" si="2"/>
         <v>199.52589097462999</v>
       </c>
+      <c r="N4">
+        <v>2764.75</v>
+      </c>
+      <c r="O4">
+        <v>254.12</v>
+      </c>
+      <c r="P4">
+        <v>194.29</v>
+      </c>
+      <c r="Q4">
+        <v>192.57</v>
+      </c>
+      <c r="R4">
+        <v>193.43</v>
+      </c>
+      <c r="S4">
+        <v>2834.84</v>
+      </c>
+      <c r="T4">
+        <v>280.49</v>
+      </c>
+      <c r="U4">
+        <v>209.55</v>
+      </c>
+      <c r="V4">
+        <v>207.89</v>
+      </c>
+      <c r="W4">
+        <f t="shared" si="3"/>
+        <v>208.72</v>
+      </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>99</v>
       </c>
@@ -586,25 +777,62 @@
         <v>184.1</v>
       </c>
       <c r="G5">
+        <v>2826.13</v>
+      </c>
+      <c r="H5">
+        <v>271.54000000000002</v>
+      </c>
+      <c r="I5">
         <v>7.3655388899999998</v>
       </c>
-      <c r="H5">
+      <c r="J5">
         <f t="shared" si="0"/>
         <v>200.42367873578999</v>
       </c>
-      <c r="I5">
+      <c r="K5">
         <v>7.3031759100000002</v>
       </c>
-      <c r="J5">
+      <c r="L5">
         <f t="shared" si="1"/>
         <v>198.72671968700999</v>
       </c>
-      <c r="K5">
+      <c r="M5">
         <f t="shared" si="2"/>
         <v>199.57519921139999</v>
       </c>
+      <c r="N5">
+        <v>2764.75</v>
+      </c>
+      <c r="O5">
+        <v>254.16</v>
+      </c>
+      <c r="P5">
+        <v>194.32</v>
+      </c>
+      <c r="Q5">
+        <v>192.62</v>
+      </c>
+      <c r="R5">
+        <v>193.47</v>
+      </c>
+      <c r="S5">
+        <v>2834.84</v>
+      </c>
+      <c r="T5">
+        <v>280.49</v>
+      </c>
+      <c r="U5">
+        <v>209.55</v>
+      </c>
+      <c r="V5">
+        <v>207.89</v>
+      </c>
+      <c r="W5">
+        <f t="shared" si="3"/>
+        <v>208.72</v>
+      </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>149</v>
       </c>
@@ -624,25 +852,62 @@
         <v>183.8</v>
       </c>
       <c r="G6">
+        <v>2825.92</v>
+      </c>
+      <c r="H6">
+        <v>271.32</v>
+      </c>
+      <c r="I6">
         <v>7.3560084000000003</v>
       </c>
-      <c r="H6">
+      <c r="J6">
         <f t="shared" si="0"/>
         <v>200.16434457240001</v>
       </c>
-      <c r="I6">
+      <c r="K6">
         <v>7.2936461799999996</v>
       </c>
-      <c r="J6">
+      <c r="L6">
         <f t="shared" si="1"/>
         <v>198.46740620397998</v>
       </c>
-      <c r="K6">
+      <c r="M6">
         <f t="shared" si="2"/>
         <v>199.31587538818999</v>
       </c>
+      <c r="N6">
+        <v>2764.45</v>
+      </c>
+      <c r="O6">
+        <v>253.93</v>
+      </c>
+      <c r="P6">
+        <v>194.29</v>
+      </c>
+      <c r="Q6">
+        <v>192.59</v>
+      </c>
+      <c r="R6">
+        <v>193.44</v>
+      </c>
+      <c r="S6">
+        <v>2834.62</v>
+      </c>
+      <c r="T6">
+        <v>280.27</v>
+      </c>
+      <c r="U6">
+        <v>209.36</v>
+      </c>
+      <c r="V6">
+        <v>207.7</v>
+      </c>
+      <c r="W6">
+        <f t="shared" si="3"/>
+        <v>208.53</v>
+      </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>199</v>
       </c>
@@ -662,22 +927,59 @@
         <v>183.9</v>
       </c>
       <c r="G7">
+        <v>2825.94</v>
+      </c>
+      <c r="H7">
+        <v>271.38</v>
+      </c>
+      <c r="I7">
         <v>7.3576023499999996</v>
       </c>
-      <c r="H7">
+      <c r="J7">
         <f t="shared" si="0"/>
         <v>200.20771754584999</v>
       </c>
-      <c r="I7">
+      <c r="K7">
         <v>7.2952401</v>
       </c>
-      <c r="J7">
+      <c r="L7">
         <f t="shared" si="1"/>
         <v>198.51077836109999</v>
       </c>
-      <c r="K7">
+      <c r="M7">
         <f t="shared" si="2"/>
         <v>199.35924795347501</v>
+      </c>
+      <c r="N7">
+        <v>2764.45</v>
+      </c>
+      <c r="O7">
+        <v>253.98</v>
+      </c>
+      <c r="P7">
+        <v>194.31</v>
+      </c>
+      <c r="Q7">
+        <v>192.61</v>
+      </c>
+      <c r="R7">
+        <v>193.46</v>
+      </c>
+      <c r="S7">
+        <v>2834.65</v>
+      </c>
+      <c r="T7">
+        <v>280.3</v>
+      </c>
+      <c r="U7">
+        <v>209.39</v>
+      </c>
+      <c r="V7">
+        <v>207.72</v>
+      </c>
+      <c r="W7">
+        <f t="shared" si="3"/>
+        <v>208.55500000000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added embedded graph to master
</commit_message>
<xml_diff>
--- a/CLUSTER-SIZES-0act-cl-n-hcl.xlsx
+++ b/CLUSTER-SIZES-0act-cl-n-hcl.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/opoku/Desktop/HCl_project_graphs_binder/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6F75C48-434F-3746-B42B-DFB2F87A5523}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47D3BA30-C5AE-BE43-BC82-750FCC47BE98}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-400" yWindow="460" windowWidth="13600" windowHeight="8620" xr2:uid="{66FEA771-CEBD-3F41-A3DD-F4748892B5D8}"/>
+    <workbookView xWindow="-2480" yWindow="460" windowWidth="13600" windowHeight="6920" xr2:uid="{66FEA771-CEBD-3F41-A3DD-F4748892B5D8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -455,8 +455,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55387CED-37BE-2A46-9802-6A940C968A22}">
   <dimension ref="A1:W7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
-      <selection activeCell="X9" sqref="X9"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -576,25 +576,25 @@
         <v>198.972068348785</v>
       </c>
       <c r="N2">
-        <v>2764.75</v>
+        <v>2764.6</v>
       </c>
       <c r="O2">
-        <v>254.19</v>
+        <v>254.15</v>
       </c>
       <c r="P2">
-        <v>194.07</v>
+        <v>194.28</v>
       </c>
       <c r="Q2">
-        <v>192.38</v>
+        <v>192.55</v>
       </c>
       <c r="R2">
-        <v>193.23</v>
+        <v>193.42</v>
       </c>
       <c r="S2">
-        <v>2834.68</v>
+        <v>2834.57</v>
       </c>
       <c r="T2">
-        <v>280.3</v>
+        <v>280.27</v>
       </c>
       <c r="U2">
         <v>209.74</v>
@@ -627,10 +627,10 @@
         <v>183.73</v>
       </c>
       <c r="G3">
-        <v>2825.73</v>
+        <v>2825.59</v>
       </c>
       <c r="H3">
-        <v>271.13</v>
+        <v>271.02</v>
       </c>
       <c r="I3">
         <v>7.3566480800000003</v>
@@ -651,25 +651,25 @@
         <v>199.33354798030501</v>
       </c>
       <c r="N3">
-        <v>2764.75</v>
+        <v>2764.6</v>
       </c>
       <c r="O3">
-        <v>254.09</v>
+        <v>254.04</v>
       </c>
       <c r="P3">
-        <v>194.26</v>
+        <v>194.15</v>
       </c>
       <c r="Q3">
-        <v>192.56</v>
+        <v>192.46</v>
       </c>
       <c r="R3">
-        <v>193.41</v>
+        <v>193.31</v>
       </c>
       <c r="S3">
-        <v>2834.81</v>
+        <v>2834.57</v>
       </c>
       <c r="T3">
-        <v>280.45999999999998</v>
+        <v>280.27300000000002</v>
       </c>
       <c r="U3">
         <v>209.52</v>
@@ -702,10 +702,10 @@
         <v>184</v>
       </c>
       <c r="G4">
-        <v>2825.92</v>
+        <v>2825.86</v>
       </c>
       <c r="H4">
-        <v>271.32</v>
+        <v>271.29000000000002</v>
       </c>
       <c r="I4">
         <v>7.3637261199999999</v>
@@ -726,25 +726,25 @@
         <v>199.52589097462999</v>
       </c>
       <c r="N4">
-        <v>2764.75</v>
+        <v>2764.6</v>
       </c>
       <c r="O4">
-        <v>254.12</v>
+        <v>254.07</v>
       </c>
       <c r="P4">
-        <v>194.29</v>
+        <v>194.23</v>
       </c>
       <c r="Q4">
-        <v>192.57</v>
+        <v>192.52</v>
       </c>
       <c r="R4">
-        <v>193.43</v>
+        <v>193.38</v>
       </c>
       <c r="S4">
-        <v>2834.84</v>
+        <v>2834.6</v>
       </c>
       <c r="T4">
-        <v>280.49</v>
+        <v>280.3</v>
       </c>
       <c r="U4">
         <v>209.55</v>
@@ -777,10 +777,10 @@
         <v>184.1</v>
       </c>
       <c r="G5">
-        <v>2826.13</v>
+        <v>2825.9</v>
       </c>
       <c r="H5">
-        <v>271.54000000000002</v>
+        <v>271.3</v>
       </c>
       <c r="I5">
         <v>7.3655388899999998</v>
@@ -801,25 +801,25 @@
         <v>199.57519921139999</v>
       </c>
       <c r="N5">
-        <v>2764.75</v>
+        <v>2764.6</v>
       </c>
       <c r="O5">
-        <v>254.16</v>
+        <v>254.1</v>
       </c>
       <c r="P5">
-        <v>194.32</v>
+        <v>194.25</v>
       </c>
       <c r="Q5">
-        <v>192.62</v>
+        <v>192.54</v>
       </c>
       <c r="R5">
-        <v>193.47</v>
+        <v>193.39</v>
       </c>
       <c r="S5">
-        <v>2834.84</v>
+        <v>2834.6</v>
       </c>
       <c r="T5">
-        <v>280.49</v>
+        <v>280.3</v>
       </c>
       <c r="U5">
         <v>209.55</v>
@@ -852,10 +852,10 @@
         <v>183.8</v>
       </c>
       <c r="G6">
-        <v>2825.92</v>
+        <v>2825.86</v>
       </c>
       <c r="H6">
-        <v>271.32</v>
+        <v>271.29000000000002</v>
       </c>
       <c r="I6">
         <v>7.3560084000000003</v>
@@ -876,25 +876,25 @@
         <v>199.31587538818999</v>
       </c>
       <c r="N6">
-        <v>2764.45</v>
+        <v>2764.36</v>
       </c>
       <c r="O6">
-        <v>253.93</v>
+        <v>253.85</v>
       </c>
       <c r="P6">
-        <v>194.29</v>
+        <v>194.05</v>
       </c>
       <c r="Q6">
-        <v>192.59</v>
+        <v>192.31</v>
       </c>
       <c r="R6">
-        <v>193.44</v>
+        <v>193.17</v>
       </c>
       <c r="S6">
-        <v>2834.62</v>
+        <v>2834.56</v>
       </c>
       <c r="T6">
-        <v>280.27</v>
+        <v>280.25</v>
       </c>
       <c r="U6">
         <v>209.36</v>
@@ -927,10 +927,10 @@
         <v>183.9</v>
       </c>
       <c r="G7">
-        <v>2825.94</v>
+        <v>2825.9</v>
       </c>
       <c r="H7">
-        <v>271.38</v>
+        <v>271.3</v>
       </c>
       <c r="I7">
         <v>7.3576023499999996</v>
@@ -951,25 +951,25 @@
         <v>199.35924795347501</v>
       </c>
       <c r="N7">
-        <v>2764.45</v>
+        <v>2764.36</v>
       </c>
       <c r="O7">
-        <v>253.98</v>
+        <v>253.88</v>
       </c>
       <c r="P7">
-        <v>194.31</v>
+        <v>194.08</v>
       </c>
       <c r="Q7">
-        <v>192.61</v>
+        <v>192.35</v>
       </c>
       <c r="R7">
-        <v>193.46</v>
+        <v>193.2</v>
       </c>
       <c r="S7">
-        <v>2834.65</v>
+        <v>2834.57</v>
       </c>
       <c r="T7">
-        <v>280.3</v>
+        <v>280.27</v>
       </c>
       <c r="U7">
         <v>209.39</v>

</xml_diff>

<commit_message>
made changes to some graphs
</commit_message>
<xml_diff>
--- a/CLUSTER-SIZES-0act-cl-n-hcl.xlsx
+++ b/CLUSTER-SIZES-0act-cl-n-hcl.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/opoku/Desktop/HCl_project_graphs_binder/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47D3BA30-C5AE-BE43-BC82-750FCC47BE98}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C2BACCC-95EF-F74B-842B-1D0505892046}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-2480" yWindow="460" windowWidth="13600" windowHeight="6920" xr2:uid="{66FEA771-CEBD-3F41-A3DD-F4748892B5D8}"/>
+    <workbookView xWindow="0" yWindow="840" windowWidth="13120" windowHeight="7560" xr2:uid="{66FEA771-CEBD-3F41-A3DD-F4748892B5D8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -455,8 +455,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55387CED-37BE-2A46-9802-6A940C968A22}">
   <dimension ref="A1:W7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -609,7 +609,7 @@
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A3">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B3">
         <v>2755.14</v>
@@ -684,7 +684,7 @@
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A4">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B4">
         <v>2755.4</v>
@@ -759,7 +759,7 @@
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A5">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B5">
         <v>2755.55</v>
@@ -834,7 +834,7 @@
     </row>
     <row r="6" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A6">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="B6">
         <v>2755</v>
@@ -909,7 +909,7 @@
     </row>
     <row r="7" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A7">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="B7">
         <v>2755.3</v>
@@ -984,5 +984,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>